<commit_message>
correct jst smd connector part number
the ordered connector is the wrong type,
it is flat on the pcb when it should be standing up
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -89,10 +89,10 @@
     <t>2.2 A</t>
   </si>
   <si>
-    <t>JST connector 2mm, 2way, right angle</t>
-  </si>
-  <si>
-    <t>http://uk.farnell.com/jst-japan-solderless-terminals/s2b-ph-sm4-tb-lf-sn/connector-header-smt-r-a-2mm-2way/dp/9492615</t>
+    <t>JST connector 2mm, 2way</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/jst-japan-solderless-terminals/b2b-ph-sm4-tb-lf-sn/connector-header-smt-2mm-2way/dp/9492534?Ntt=9492534</t>
   </si>
   <si>
     <t>JST housing, 2way plug</t>
@@ -448,7 +448,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+      <selection activeCell="A15" activeCellId="0" pane="topLeft" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -627,8 +627,8 @@
       <c r="D15" s="1" t="n">
         <v>2.31</v>
       </c>
-      <c r="E15" s="5" t="n">
-        <v>9492615</v>
+      <c r="E15" s="1" t="n">
+        <v>9492534</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>25</v>

</xml_diff>